<commit_message>
3/17 re-run simulations, set SAM bias for Row 8 Tamb = 0.  Still need to update figures.
</commit_message>
<xml_diff>
--- a/Analysis/SAM_00 summary.xlsx
+++ b/Analysis/SAM_00 summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB5D740-73ED-4FA2-9E86-06786FEB817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD3042B-2C88-4E6E-8E14-74552E684D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6360" windowWidth="29040" windowHeight="15840" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="4" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="37">
   <si>
     <t>Column1</t>
   </si>
@@ -197,12 +197,15 @@
   <si>
     <t>&lt;- Mono baseline</t>
   </si>
+  <si>
+    <t>***  NEED TO UPDATE RAW DATA AND PLOTS ***</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +225,19 @@
       <u/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -247,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -255,6 +271,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -25908,8 +25926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8C243-CD6D-4F25-B152-197695A0DCE2}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25961,35 +25979,41 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>-0.83</v>
-      </c>
-      <c r="E3">
-        <v>1.22</v>
-      </c>
-      <c r="I3">
+      <c r="D3" s="6">
+        <v>-0.03</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L3">
-        <v>-0.69</v>
-      </c>
-      <c r="M3">
-        <v>1.27</v>
+      <c r="L3" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1.28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -26002,11 +26026,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>-0.51</v>
-      </c>
-      <c r="E4">
-        <v>1.33</v>
+      <c r="D4" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4.07</v>
       </c>
       <c r="I4">
         <v>8</v>
@@ -26017,49 +26041,43 @@
       <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="L4">
-        <v>-0.44</v>
-      </c>
-      <c r="M4">
-        <v>2.0299999999999998</v>
+      <c r="L4" s="5">
+        <v>13.4</v>
+      </c>
+      <c r="M4" s="5">
+        <v>11.8</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="7">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2">
-        <v>-0.38</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="D5" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="I5" s="7">
         <v>8</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="2">
-        <v>-0.4</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
+      <c r="L5" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1.51</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -26072,11 +26090,11 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>-0.28999999999999998</v>
-      </c>
-      <c r="E6">
-        <v>1.52</v>
+      <c r="D6" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3.61</v>
       </c>
       <c r="I6">
         <v>8</v>
@@ -26088,10 +26106,10 @@
         <v>13</v>
       </c>
       <c r="L6" s="5">
-        <v>-0.24</v>
+        <v>11.94</v>
       </c>
       <c r="M6" s="5">
-        <v>1.98</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -26104,11 +26122,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2.2999999999999998</v>
+      <c r="D7" s="5">
+        <v>2.83</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2.34</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -26123,10 +26141,10 @@
         <v>12</v>
       </c>
       <c r="L7" s="5">
-        <v>3.09</v>
+        <v>3.94</v>
       </c>
       <c r="M7" s="5">
-        <v>3.47</v>
+        <v>3.6</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
@@ -26142,11 +26160,11 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
-        <v>1.83</v>
-      </c>
-      <c r="E8">
-        <v>1.66</v>
+      <c r="D8" s="5">
+        <v>6.16</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.07</v>
       </c>
       <c r="I8">
         <v>4</v>
@@ -26158,10 +26176,10 @@
         <v>13</v>
       </c>
       <c r="L8" s="5">
-        <v>3.13</v>
+        <v>14.08</v>
       </c>
       <c r="M8" s="5">
-        <v>3.28</v>
+        <v>11.35</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -26174,11 +26192,11 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9">
-        <v>1.89</v>
-      </c>
-      <c r="E9">
-        <v>1.86</v>
+      <c r="D9" s="5">
+        <v>3.37</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.64</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -26189,6 +26207,8 @@
       <c r="K9" t="s">
         <v>12</v>
       </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -26200,11 +26220,11 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>-0.12</v>
-      </c>
-      <c r="E10">
-        <v>1.26</v>
+      <c r="D10" s="5">
+        <v>0.69</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.27</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
@@ -26218,11 +26238,11 @@
       <c r="K10" t="s">
         <v>12</v>
       </c>
-      <c r="L10">
-        <v>0.25</v>
-      </c>
-      <c r="M10">
-        <v>1.54</v>
+      <c r="L10" s="5">
+        <v>1.02</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1.59</v>
       </c>
       <c r="N10" t="s">
         <v>27</v>
@@ -26238,11 +26258,11 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>0.16</v>
-      </c>
-      <c r="E11">
-        <v>1.43</v>
+      <c r="D11" s="5">
+        <v>6.39</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.92</v>
       </c>
       <c r="H11" t="s">
         <v>32</v>
@@ -26256,11 +26276,11 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-      <c r="L11">
-        <v>0.44</v>
-      </c>
-      <c r="M11">
-        <v>1.39</v>
+      <c r="L11" s="5">
+        <v>13.54</v>
+      </c>
+      <c r="M11" s="5">
+        <v>12.88</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -26273,11 +26293,11 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12">
-        <v>-4.7699999999999996</v>
-      </c>
-      <c r="E12">
-        <v>0.64</v>
+      <c r="D12" s="5">
+        <v>-1.76</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.75</v>
       </c>
       <c r="F12" t="s">
         <v>28</v>
@@ -26291,6 +26311,8 @@
       <c r="K12" t="s">
         <v>12</v>
       </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -26302,11 +26324,11 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13">
-        <v>-7.94</v>
-      </c>
-      <c r="E13">
-        <v>3.46</v>
+      <c r="D13" s="5">
+        <v>-7.25</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3.5</v>
       </c>
       <c r="F13" t="s">
         <v>29</v>
@@ -26320,6 +26342,8 @@
       <c r="K13" t="s">
         <v>12</v>
       </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -26331,22 +26355,32 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>-2.5499999999999998</v>
-      </c>
-      <c r="E14">
-        <v>0.74</v>
-      </c>
+      <c r="D14" s="5">
+        <v>-3.31</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>22</v>
       </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>23</v>
       </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -26358,11 +26392,11 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17">
-        <v>-1.48</v>
-      </c>
-      <c r="E17">
-        <v>1.58</v>
+      <c r="D17" s="5">
+        <v>-0.68</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.59</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -26376,11 +26410,11 @@
       <c r="K17" t="s">
         <v>12</v>
       </c>
-      <c r="L17">
-        <v>-0.81</v>
-      </c>
-      <c r="M17">
-        <v>2.62</v>
+      <c r="L17" s="5">
+        <v>-0.01</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2.64</v>
       </c>
       <c r="N17" t="s">
         <v>26</v>
@@ -26396,11 +26430,11 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18">
-        <v>-2.4</v>
-      </c>
-      <c r="E18">
-        <v>1.02</v>
+      <c r="D18" s="5">
+        <v>2.82</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2.76</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -26411,11 +26445,11 @@
       <c r="K18" t="s">
         <v>13</v>
       </c>
-      <c r="L18">
-        <v>-1.37</v>
-      </c>
-      <c r="M18">
-        <v>2.62</v>
+      <c r="L18" s="5">
+        <v>10.24</v>
+      </c>
+      <c r="M18" s="5">
+        <v>10.41</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -26428,11 +26462,11 @@
       <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D19">
-        <v>-2.36</v>
-      </c>
-      <c r="E19">
-        <v>1.1100000000000001</v>
+      <c r="D19" s="5">
+        <v>-1.3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.17</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -26443,6 +26477,8 @@
       <c r="K19" t="s">
         <v>12</v>
       </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -26454,11 +26490,11 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
-      <c r="D20">
-        <v>-3.8</v>
-      </c>
-      <c r="E20">
-        <v>1.02</v>
+      <c r="D20" s="5">
+        <v>-3.02</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1.03</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
@@ -26472,11 +26508,11 @@
       <c r="K20" t="s">
         <v>12</v>
       </c>
-      <c r="L20">
-        <v>-4.12</v>
-      </c>
-      <c r="M20">
-        <v>1.3</v>
+      <c r="L20" s="5">
+        <v>-3.34</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1.31</v>
       </c>
       <c r="N20" t="s">
         <v>27</v>
@@ -26492,11 +26528,11 @@
       <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="D21">
-        <v>-4.37</v>
-      </c>
-      <c r="E21">
-        <v>1.0900000000000001</v>
+      <c r="D21" s="5">
+        <v>1.81</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3.48</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -26507,11 +26543,11 @@
       <c r="K21" t="s">
         <v>13</v>
       </c>
-      <c r="L21">
-        <v>-4.26</v>
-      </c>
-      <c r="M21">
-        <v>1.27</v>
+      <c r="L21" s="5">
+        <v>8.36</v>
+      </c>
+      <c r="M21" s="5">
+        <v>12.07</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -26524,11 +26560,11 @@
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22">
-        <v>-8.1300000000000008</v>
-      </c>
-      <c r="E22">
-        <v>1.1100000000000001</v>
+      <c r="D22" s="5">
+        <v>-7.29</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1.3</v>
       </c>
       <c r="F22" t="s">
         <v>28</v>
@@ -26544,11 +26580,16 @@
       <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D23">
-        <v>-7.08</v>
-      </c>
-      <c r="E23">
-        <v>0.85</v>
+      <c r="D23" s="5">
+        <v>-6.33</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Minor update to figures for 4/25 PVPG quarterly review.
</commit_message>
<xml_diff>
--- a/Analysis/SAM_00 summary.xlsx
+++ b/Analysis/SAM_00 summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F9A745-EA2B-4080-A200-056500ED7986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94FE443-B1DC-4099-9B8B-9A902A2EC80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24645,12 +24645,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.23903</cdr:x>
-      <cdr:y>0.6454</cdr:y>
+      <cdr:x>0.24293</cdr:x>
+      <cdr:y>0.49995</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.48471</cdr:x>
-      <cdr:y>0.7499</cdr:y>
+      <cdr:x>0.48861</cdr:x>
+      <cdr:y>0.60445</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -24665,8 +24665,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1009496" y="1533164"/>
-          <a:ext cx="1037601" cy="248243"/>
+          <a:off x="1031624" y="1195724"/>
+          <a:ext cx="1043299" cy="249931"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -26126,8 +26126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8C243-CD6D-4F25-B152-197695A0DCE2}">
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF49" sqref="AF49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Initial Method 3 analysis with calculated unshaded Grear
</commit_message>
<xml_diff>
--- a/Analysis/SAM_00 summary.xlsx
+++ b/Analysis/SAM_00 summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539C969-EC1F-4933-89DE-772E9CD319BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70DB454-215D-4AF9-908B-CB10B659E32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-6360" windowWidth="29040" windowHeight="15840" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="147">
   <si>
     <t>Column1</t>
   </si>
@@ -516,15 +516,28 @@
   <si>
     <t>2022-05-29 18:00:00-07:00</t>
   </si>
+  <si>
+    <t>Method 1</t>
+  </si>
+  <si>
+    <t>Method 2</t>
+  </si>
+  <si>
+    <t>Method 4</t>
+  </si>
+  <si>
+    <t>Monofacial (baseline)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +592,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -600,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -615,6 +637,27 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26171,10 +26214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8C243-CD6D-4F25-B152-197695A0DCE2}">
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -26846,6 +26889,129 @@
       <c r="J44" s="3" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="28.8">
+      <c r="B71" s="13">
+        <v>8</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="E71" s="11">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="10">
+        <v>4</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D72" s="11">
+        <v>1.69</v>
+      </c>
+      <c r="E72" s="11">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="10">
+        <v>4</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="11">
+        <v>-0.47</v>
+      </c>
+      <c r="E73" s="11">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="10">
+        <v>4</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D74" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="E74" s="11">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="10">
+        <v>2</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" s="11">
+        <v>-0.23</v>
+      </c>
+      <c r="E76" s="11">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="10">
+        <v>2</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D77" s="11">
+        <v>-2.63</v>
+      </c>
+      <c r="E77" s="11">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="10">
+        <v>2</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D78" s="11">
+        <v>-1.75</v>
+      </c>
+      <c r="E78" s="11">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79" s="2"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Runs for P07 and new P11 run with monthly albedo and look at min of hydra. POA input runs still failing in pySAM.
</commit_message>
<xml_diff>
--- a/Analysis/SAM_00 summary.xlsx
+++ b/Analysis/SAM_00 summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C051042-009A-4B67-BBE8-7955CA602EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96A71E-4788-484E-B02D-CFC263AB040F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-6360" windowWidth="29040" windowHeight="15840" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="4" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="157">
   <si>
     <t>Column1</t>
   </si>
@@ -544,7 +544,22 @@
     <t>SAMTMYA01 model results - Row 2+4</t>
   </si>
   <si>
-    <t>SAMP00 model results - Row 2+4</t>
+    <t>SAMP11 (CM11 POA and monthly albedo) - row 2+4</t>
+  </si>
+  <si>
+    <t>-0.00</t>
+  </si>
+  <si>
+    <t>Method4Min</t>
+  </si>
+  <si>
+    <t>&lt;- Method 4_min</t>
+  </si>
+  <si>
+    <t>SAMP07 (CM11 POA and high freq albedo) - row 2+4</t>
+  </si>
+  <si>
+    <t>SAMP00 (RefCell POA, high frequency albedo)</t>
   </si>
 </sst>
 </file>
@@ -648,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -683,6 +698,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -19640,13 +19661,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>17145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19683,7 +19704,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>439474</xdr:colOff>
+      <xdr:colOff>435664</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>73503</xdr:rowOff>
     </xdr:to>
@@ -19739,13 +19760,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>150495</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>17145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19777,13 +19798,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>174966</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>75321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>108292</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>100086</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19815,13 +19836,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>116205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19853,13 +19874,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>140970</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19891,13 +19912,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>257158</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>43082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>200996</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>70118</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19934,7 +19955,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>208390</xdr:colOff>
+      <xdr:colOff>212200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>111084</xdr:rowOff>
     </xdr:to>
@@ -19995,9 +20016,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>93675</xdr:colOff>
+      <xdr:colOff>97485</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>55908</xdr:rowOff>
+      <xdr:rowOff>59718</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -20051,13 +20072,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>165653</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>118028</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>65515</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -20089,13 +20110,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>173935</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>173935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>256927</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>22198</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26549,10 +26570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8C243-CD6D-4F25-B152-197695A0DCE2}">
-  <dimension ref="A1:Z98"/>
+  <dimension ref="A1:Z113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -26841,7 +26862,7 @@
         <v>1.84</v>
       </c>
       <c r="I10" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -26908,7 +26929,7 @@
         <v>12</v>
       </c>
       <c r="L12" s="5">
-        <v>-0.18</v>
+        <v>0</v>
       </c>
       <c r="M12" s="5">
         <v>1.62</v>
@@ -26946,7 +26967,7 @@
         <v>12</v>
       </c>
       <c r="L13" s="4">
-        <v>0.04</v>
+        <v>0.22</v>
       </c>
       <c r="M13" s="4">
         <v>1.85</v>
@@ -26981,10 +27002,10 @@
         <v>12</v>
       </c>
       <c r="L14" s="4">
-        <v>5.68</v>
+        <v>5.88</v>
       </c>
       <c r="M14" s="4">
-        <v>3.29</v>
+        <v>3.3</v>
       </c>
       <c r="N14" t="s">
         <v>19</v>
@@ -27019,7 +27040,7 @@
         <v>12</v>
       </c>
       <c r="L15" s="4">
-        <v>-1.18</v>
+        <v>-1.01</v>
       </c>
       <c r="M15" s="4">
         <v>1.39</v>
@@ -27041,254 +27062,549 @@
         <v>12</v>
       </c>
       <c r="L16" s="8">
-        <v>-0.51</v>
+        <v>-0.32</v>
       </c>
       <c r="M16" s="4">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="N16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
+      <c r="I18" s="17" t="s">
+        <v>151</v>
+      </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="I20" s="1">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="N20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="I22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22">
+        <v>5.95</v>
+      </c>
+      <c r="M22">
+        <v>3.47</v>
+      </c>
+      <c r="N22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="I23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="4">
+        <v>-1.01</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1.39</v>
+      </c>
+      <c r="N23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="2"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-    </row>
-    <row r="26" spans="1:13" ht="23.4">
-      <c r="J26" s="3" t="s">
+      <c r="I24" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="4">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="I25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J25" t="s">
+        <v>153</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1.41</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="N25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="I26" s="2"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="I27" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="I29" s="1">
+        <v>8</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="18">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1.68</v>
+      </c>
+      <c r="N29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="I31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31">
+        <v>5.97</v>
+      </c>
+      <c r="M31">
+        <v>3.48</v>
+      </c>
+      <c r="N31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="I32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="4">
+        <v>-1.02</v>
+      </c>
+      <c r="M32" s="4">
+        <v>1.39</v>
+      </c>
+      <c r="N32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="9:14">
+      <c r="I33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J33" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="4">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="M33" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="N33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="9:14">
+      <c r="I34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J34" t="s">
+        <v>153</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="M34" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="N34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="9:14">
+      <c r="I35" s="2"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="9:14">
+      <c r="I36" s="2"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+    </row>
+    <row r="37" spans="9:14">
+      <c r="I37" s="2"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="9:14">
+      <c r="I38" s="2"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="9:14">
+      <c r="I39" s="2"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="9:14">
+      <c r="I40" s="2"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="9:14" ht="23.4">
+      <c r="J41" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="10:10" ht="23.4">
-      <c r="J45" s="3" t="s">
+    <row r="60" spans="10:10" ht="23.4">
+      <c r="J60" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="10:10" ht="23.4">
-      <c r="J62" s="3" t="s">
+    <row r="77" spans="10:10" ht="23.4">
+      <c r="J77" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="2:7">
-      <c r="D88" t="s">
+    <row r="103" spans="2:7">
+      <c r="D103" t="s">
         <v>144</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F103" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G88" s="4"/>
-    </row>
-    <row r="89" spans="2:7">
-      <c r="B89" s="15" t="s">
+      <c r="G103" s="4"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C104" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D104" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="E104" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="16" t="s">
+      <c r="F104" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G89" s="16" t="s">
+      <c r="G104" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="28.8">
-      <c r="B90" s="10">
+    <row r="105" spans="2:7" ht="28.8">
+      <c r="B105" s="10">
         <v>8</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C105" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D90" s="14">
+      <c r="D105" s="14">
         <v>0</v>
       </c>
-      <c r="E90" s="11">
+      <c r="E105" s="11">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F90" s="14">
+      <c r="F105" s="14">
         <v>-0.01</v>
       </c>
-      <c r="G90" s="11">
+      <c r="G105" s="11">
         <v>1.05</v>
       </c>
     </row>
-    <row r="91" spans="2:7">
-      <c r="B91" s="10">
+    <row r="106" spans="2:7">
+      <c r="B106" s="10">
         <v>4</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C106" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D91" s="11">
+      <c r="D106" s="11">
         <v>1.19</v>
       </c>
-      <c r="E91" s="11">
+      <c r="E106" s="11">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F91" s="11">
+      <c r="F106" s="11">
         <v>1.69</v>
       </c>
-      <c r="G91" s="11">
+      <c r="G106" s="11">
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="92" spans="2:7">
-      <c r="B92" s="10">
+    <row r="107" spans="2:7">
+      <c r="B107" s="10">
         <v>4</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C107" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D92" s="11">
+      <c r="D107" s="11">
         <v>-0.24</v>
       </c>
-      <c r="E92" s="11">
+      <c r="E107" s="11">
         <v>1.71</v>
       </c>
-      <c r="F92" s="11">
+      <c r="F107" s="11">
         <v>-0.47</v>
       </c>
-      <c r="G92" s="11">
+      <c r="G107" s="11">
         <v>1.33</v>
       </c>
     </row>
-    <row r="93" spans="2:7">
-      <c r="B93" s="10">
+    <row r="108" spans="2:7">
+      <c r="B108" s="10">
         <v>4</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C108" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D93" s="12">
+      <c r="D108" s="12">
         <v>0.34</v>
       </c>
-      <c r="E93" s="11">
+      <c r="E108" s="11">
         <v>0.96</v>
       </c>
-      <c r="F93" s="12">
+      <c r="F108" s="12">
         <v>0.18</v>
       </c>
-      <c r="G93" s="11">
+      <c r="G108" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="94" spans="2:7">
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-    </row>
-    <row r="95" spans="2:7">
-      <c r="B95" s="10">
+    <row r="109" spans="2:7">
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" s="10">
         <v>2</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C110" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D95" s="11">
+      <c r="D110" s="11">
         <v>-0.6</v>
       </c>
-      <c r="E95" s="11">
+      <c r="E110" s="11">
         <v>1.59</v>
       </c>
-      <c r="F95" s="11">
+      <c r="F110" s="11">
         <v>-0.23</v>
       </c>
-      <c r="G95" s="11">
+      <c r="G110" s="11">
         <v>1.8</v>
       </c>
     </row>
-    <row r="96" spans="2:7">
-      <c r="B96" s="10">
+    <row r="111" spans="2:7">
+      <c r="B111" s="10">
         <v>2</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C111" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D96" s="11">
+      <c r="D111" s="11">
         <v>-2.52</v>
       </c>
-      <c r="E96" s="11">
+      <c r="E111" s="11">
         <v>1.23</v>
       </c>
-      <c r="F96" s="11">
+      <c r="F111" s="11">
         <v>-2.63</v>
       </c>
-      <c r="G96" s="11">
+      <c r="G111" s="11">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
-      <c r="B97" s="10">
+    <row r="112" spans="2:7">
+      <c r="B112" s="10">
         <v>2</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C112" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D97" s="11">
+      <c r="D112" s="11">
         <v>-1.69</v>
       </c>
-      <c r="E97" s="11">
+      <c r="E112" s="11">
         <v>1.22</v>
       </c>
-      <c r="F97" s="11">
+      <c r="F112" s="11">
         <v>-1.75</v>
       </c>
-      <c r="G97" s="11">
+      <c r="G112" s="11">
         <v>1.06</v>
       </c>
     </row>
-    <row r="98" spans="2:7">
-      <c r="B98" s="2"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
+    <row r="113" spans="2:6">
+      <c r="B113" s="2"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
P00 - POA reference cell. Requires small horizon shading value in .json files
</commit_message>
<xml_diff>
--- a/Analysis/SAM_00 summary.xlsx
+++ b/Analysis/SAM_00 summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96A71E-4788-484E-B02D-CFC263AB040F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD9D40-E4A9-4D55-AEAF-1C396A1160D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-6360" windowWidth="29040" windowHeight="15840" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26573,7 +26573,7 @@
   <dimension ref="A1:Z113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>